<commit_message>
Update a specific story and update author completely finished, added icons, **php valdation**
</commit_message>
<xml_diff>
--- a/excel/NewsWebsiteData.xlsx
+++ b/excel/NewsWebsiteData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iadt-my.sharepoint.com/personal/n00212101_iadt_ie/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\Liam's_Site\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{B39FE80D-ABB7-469E-A74C-97D0C9224083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D7D699C-9D98-455B-AFA3-6B8605DD05A2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF4009C-8B05-4449-AC4F-927EDB524C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24300" yWindow="3195" windowWidth="25665" windowHeight="17550" activeTab="1" xr2:uid="{567F56AA-62DD-44B9-904D-1C9B922C9F06}"/>
+    <workbookView xWindow="26595" yWindow="1605" windowWidth="25665" windowHeight="17550" xr2:uid="{567F56AA-62DD-44B9-904D-1C9B922C9F06}"/>
   </bookViews>
   <sheets>
     <sheet name="articles" sheetId="2" r:id="rId1"/>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8278549C-76E8-4CF1-9D79-21D725479148}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4753B9BE-E19F-4FD3-B605-F162E9CEDDC0}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2105,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -2120,7 +2122,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>92</v>
       </c>
@@ -2135,7 +2139,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>93</v>
       </c>
@@ -2150,7 +2156,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>158</v>
       </c>
@@ -2165,7 +2173,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>81</v>
       </c>
@@ -2180,7 +2190,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>82</v>
       </c>
@@ -2195,7 +2207,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>84</v>
       </c>
@@ -2228,7 +2242,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,7 +2263,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
       <c r="B2" s="16" t="s">
         <v>11</v>
       </c>
@@ -2258,7 +2274,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -2267,7 +2285,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
       <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
@@ -2276,7 +2296,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
       <c r="B5" s="16" t="s">
         <v>14</v>
       </c>
@@ -2285,7 +2307,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
       <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
@@ -2294,7 +2318,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="17">
+        <v>6</v>
+      </c>
       <c r="B7" s="18" t="s">
         <v>16</v>
       </c>
@@ -2303,7 +2329,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2329,6 +2357,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037E36E452A7B42409B0F9EDF97FE4A0C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c39eb84205d6736577d655e784296b96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4c455e83-caa3-4e24-9d93-6827f1c48133" xmlns:ns4="41cd6071-ad8c-4a15-8404-f6f854c2da9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="07e976836291c002bf374e9d3969d760" ns3:_="" ns4:_="">
     <xsd:import namespace="4c455e83-caa3-4e24-9d93-6827f1c48133"/>
@@ -2551,15 +2588,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2567,6 +2595,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92B50D1B-96AA-4443-A0A9-3223C65A1E5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0CA4A7C-FFC4-4357-8242-F77F3C898F26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2581,14 +2617,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92B50D1B-96AA-4443-A0A9-3223C65A1E5F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Final push for presentation!
</commit_message>
<xml_diff>
--- a/excel/NewsWebsiteData.xlsx
+++ b/excel/NewsWebsiteData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\Liam's_Site\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF4009C-8B05-4449-AC4F-927EDB524C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF3DAFE-8098-4773-B6E7-F83CD8137BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26595" yWindow="1605" windowWidth="25665" windowHeight="17550" xr2:uid="{567F56AA-62DD-44B9-904D-1C9B922C9F06}"/>
+    <workbookView xWindow="23760" yWindow="11355" windowWidth="25665" windowHeight="17550" xr2:uid="{567F56AA-62DD-44B9-904D-1C9B922C9F06}"/>
   </bookViews>
   <sheets>
     <sheet name="articles" sheetId="2" r:id="rId1"/>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8278549C-76E8-4CF1-9D79-21D725479148}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,6 +2366,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037E36E452A7B42409B0F9EDF97FE4A0C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c39eb84205d6736577d655e784296b96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4c455e83-caa3-4e24-9d93-6827f1c48133" xmlns:ns4="41cd6071-ad8c-4a15-8404-f6f854c2da9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="07e976836291c002bf374e9d3969d760" ns3:_="" ns4:_="">
     <xsd:import namespace="4c455e83-caa3-4e24-9d93-6827f1c48133"/>
@@ -2588,12 +2594,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92B50D1B-96AA-4443-A0A9-3223C65A1E5F}">
   <ds:schemaRefs>
@@ -2603,6 +2603,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B7414C7-F4FF-49FF-887E-780CBBE5204C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="41cd6071-ad8c-4a15-8404-f6f854c2da9a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4c455e83-caa3-4e24-9d93-6827f1c48133"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0CA4A7C-FFC4-4357-8242-F77F3C898F26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2619,21 +2636,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B7414C7-F4FF-49FF-887E-780CBBE5204C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="41cd6071-ad8c-4a15-8404-f6f854c2da9a"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4c455e83-caa3-4e24-9d93-6827f1c48133"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>